<commit_message>
Uploaded Processed LST Charts - Visor V.0.9.4
</commit_message>
<xml_diff>
--- a/Glaciers_Tables/AGASSIZ_BOLADOS/AGASSIZ_BOLADOS_LST.xlsx
+++ b/Glaciers_Tables/AGASSIZ_BOLADOS/AGASSIZ_BOLADOS_LST.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/f_camacho10_uniandes_edu_co/Documents/Copernicus_Master_Olomouc_Documents/Thesis/Github/PatagonianGlaciers/Tables/AGASSIZ_BOLADOS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/f_camacho10_uniandes_edu_co/Documents/Copernicus_Master_Olomouc_Documents/Thesis/Github/PatagonianGlaciers/Glaciers_Tables/AGASSIZ_BOLADOS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="165" documentId="8_{B3B5BF9E-F017-4281-93B8-14A2DBF4A79A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9475C2B6-7D02-4C7C-BE8F-7CA84A128632}"/>
+  <xr:revisionPtr revIDLastSave="172" documentId="8_{B3B5BF9E-F017-4281-93B8-14A2DBF4A79A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB19374C-9906-4241-98AD-5190526E2A37}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AGASSIZ_BOLADOS_GLACIERAREA" sheetId="1" r:id="rId1"/>
@@ -908,7 +908,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr algn="r">
-                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="700" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -1009,8 +1009,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="3.7499781277340334E-2"/>
-                  <c:y val="0.36541666666666667"/>
+                  <c:x val="4.9416447944007E-2"/>
+                  <c:y val="0.35583333333333333"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -1019,7 +1019,7 @@
                   <a:lstStyle/>
                   <a:p>
                     <a:pPr>
-                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:defRPr sz="700" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                         <a:solidFill>
                           <a:schemeClr val="tx1">
                             <a:lumMod val="65000"/>
@@ -1032,35 +1032,35 @@
                       </a:defRPr>
                     </a:pPr>
                     <a:r>
-                      <a:rPr lang="en-US" baseline="0">
+                      <a:rPr lang="en-US" sz="700" baseline="0">
                         <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                         <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                       </a:rPr>
                       <a:t>y = 0.7562x - 3.7196</a:t>
                     </a:r>
                     <a:br>
-                      <a:rPr lang="en-US" baseline="0">
+                      <a:rPr lang="en-US" sz="700" baseline="0">
                         <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                         <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                       </a:rPr>
                     </a:br>
                     <a:r>
-                      <a:rPr lang="en-US" baseline="0">
+                      <a:rPr lang="en-US" sz="700" baseline="0">
                         <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                         <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <a:t>ȳ = -1.451</a:t>
+                      <a:t>ȳ = -1.45</a:t>
                     </a:r>
                   </a:p>
                   <a:p>
                     <a:pPr>
-                      <a:defRPr>
+                      <a:defRPr sz="700">
                         <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                         <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                       </a:defRPr>
                     </a:pPr>
                     <a:r>
-                      <a:rPr lang="en-US" baseline="0">
+                      <a:rPr lang="en-US" sz="700" baseline="0">
                         <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                         <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                       </a:rPr>
@@ -1069,19 +1069,19 @@
                   </a:p>
                   <a:p>
                     <a:pPr>
-                      <a:defRPr>
+                      <a:defRPr sz="700">
                         <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                         <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                       </a:defRPr>
                     </a:pPr>
                     <a:r>
-                      <a:rPr lang="en-US" baseline="0">
+                      <a:rPr lang="en-US" sz="700" baseline="0">
                         <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                         <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <a:t>RRMSD = 36.4%</a:t>
+                      <a:t>RMSD = 0.53</a:t>
                     </a:r>
-                    <a:endParaRPr lang="en-US">
+                    <a:endParaRPr lang="en-US" sz="700">
                       <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                       <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                     </a:endParaRPr>
@@ -1090,9 +1090,13 @@
               </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:ln w="3175">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
                 </a:ln>
                 <a:effectLst/>
               </c:spPr>
@@ -1101,7 +1105,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="700" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx1">
                           <a:lumMod val="65000"/>
@@ -1117,6 +1121,20 @@
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:cat>
             <c:strRef>

</xml_diff>